<commit_message>
Updated Curvature values using JM's methods
</commit_message>
<xml_diff>
--- a/Data/Comparing MPQ sizes and metric changes.xlsx
+++ b/Data/Comparing MPQ sizes and metric changes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Desktop/GitHub/Bruce_MPQ_Analysis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Library/Containers/com.microsoft.Excel/Data/Desktop/GitHub/Bruce_MPQ_Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C560FBD4-2804-6047-870F-2373292F6294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F215CFD-1DC5-3B4C-B00B-F9826DBF59C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{F3A4A8A6-98D9-3F48-8546-AC6A8561833A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MPQ Metric Comparissons" sheetId="4" r:id="rId1"/>
     <sheet name="DEM Scaling Issues" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -113,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +136,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,10 +183,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D564A68-4C63-1041-99F2-A3F858EAACB8}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +687,7 @@
         <v>5.0044985809999998E-2</v>
       </c>
       <c r="I5" s="9">
-        <v>1.81E-6</v>
+        <v>3.3065552899999999</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>11</v>
@@ -721,8 +724,8 @@
       <c r="H6" s="8">
         <v>6.0238317919999999E-2</v>
       </c>
-      <c r="I6" s="10">
-        <v>2.12E-6</v>
+      <c r="I6" s="9">
+        <v>5.3897394939999996</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>18</v>
@@ -759,8 +762,8 @@
       <c r="H7" s="8">
         <v>8.5429347259999996E-2</v>
       </c>
-      <c r="I7" s="10">
-        <v>1.72E-6</v>
+      <c r="I7" s="9">
+        <v>16.494041790000001</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>18</v>
@@ -911,8 +914,8 @@
       <c r="H11" s="8">
         <v>8.4818247190000001E-2</v>
       </c>
-      <c r="I11" s="10">
-        <v>2.74E-6</v>
+      <c r="I11" s="9">
+        <v>3.951547315</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>18</v>
@@ -949,8 +952,8 @@
       <c r="H12" s="8">
         <v>5.5361324939999998E-2</v>
       </c>
-      <c r="I12" s="10">
-        <v>1.6999999999999999E-7</v>
+      <c r="I12" s="9">
+        <v>2.658635834</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>11</v>
@@ -987,8 +990,8 @@
       <c r="H13" s="8">
         <v>6.238559934E-2</v>
       </c>
-      <c r="I13" s="10">
-        <v>-1.3999999999999999E-6</v>
+      <c r="I13" s="9">
+        <v>11.362216119999999</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updated curvature results included in these files
</commit_message>
<xml_diff>
--- a/Data/Comparing MPQ sizes and metric changes.xlsx
+++ b/Data/Comparing MPQ sizes and metric changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Library/Containers/com.microsoft.Excel/Data/Desktop/GitHub/Bruce_MPQ_Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F215CFD-1DC5-3B4C-B00B-F9826DBF59C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B76F8A-9DA1-344F-897E-8E0A96456814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{F3A4A8A6-98D9-3F48-8546-AC6A8561833A}"/>
   </bookViews>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D564A68-4C63-1041-99F2-A3F858EAACB8}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -953,7 +953,7 @@
         <v>5.5361324939999998E-2</v>
       </c>
       <c r="I12" s="9">
-        <v>2.658635834</v>
+        <v>0.64262741000000001</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>11</v>
@@ -991,7 +991,7 @@
         <v>6.238559934E-2</v>
       </c>
       <c r="I13" s="9">
-        <v>11.362216119999999</v>
+        <v>51.941000000000003</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>11</v>

</xml_diff>